<commit_message>
Update contact log template
</commit_message>
<xml_diff>
--- a/Contact Log.xlsx
+++ b/Contact Log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slovell\Documents\Paul Sheldon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DF750D-CEE5-4DDD-B103-06B16D811CDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED64230D-5B70-4370-97CA-716A72C3B89A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D891645B-2418-4F4D-AB96-6243403940A5}"/>
+    <workbookView xWindow="-20617" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{D891645B-2418-4F4D-AB96-6243403940A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <t>Regarding</t>
   </si>
   <si>
-    <t>Contact Log : Christopher Martens Law Corp</t>
+    <t>Contact Log</t>
   </si>
 </sst>
 </file>
@@ -509,16 +509,16 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.73046875" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="41" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -526,7 +526,7 @@
       <c r="C1" s="6"/>
       <c r="D1" s="7"/>
     </row>
-    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
     </row>
   </sheetData>

</xml_diff>